<commit_message>
Added clear command to calc (LabeledExpr)
</commit_message>
<xml_diff>
--- a/11_Grammars/Ti Docs/TI5x instructions.xlsx
+++ b/11_Grammars/Ti Docs/TI5x instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Projects\11_TI5x\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Projects\11_Grammars\Ti Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33338BEB-376E-4239-98ED-86CD3BD86762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886E6756-4164-48C0-BF2C-E749B7D9EFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="7020" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
+    <workbookView xWindow="24840" yWindow="3840" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions table" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -730,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -739,7 +739,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1708,7 +1707,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9793B594-CD2F-489C-A9EA-F016C26CC5A7}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9793B594-CD2F-489C-A9EA-F016C26CC5A7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -2211,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740F8AED-F224-4E04-9363-190526C87892}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q102" sqref="Q102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3407,7 +3406,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" ref="A76:A107" si="2">VALUE(MID(B76,2,2))</f>
+        <f t="shared" ref="A76:A101" si="2">VALUE(MID(B76,2,2))</f>
         <v>74</v>
       </c>
       <c r="B76" t="s">
@@ -3864,7 +3863,16 @@
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" start="4" max="11" activeRow="7" previousRow="7" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" fieldPosition="0">
+          <references count="1">
+            <reference field="3" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3885,7 +3893,7 @@
       <c r="A4" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
         <v>67</v>
       </c>
     </row>
@@ -3893,7 +3901,7 @@
       <c r="A5" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>8</v>
       </c>
     </row>
@@ -3901,7 +3909,7 @@
       <c r="A6" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
@@ -3909,7 +3917,7 @@
       <c r="A7" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
@@ -3917,7 +3925,7 @@
       <c r="A8" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>4</v>
       </c>
     </row>
@@ -3925,7 +3933,7 @@
       <c r="A9" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>1</v>
       </c>
     </row>
@@ -3933,7 +3941,7 @@
       <c r="A10" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>7</v>
       </c>
     </row>
@@ -3941,7 +3949,7 @@
       <c r="A11" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11">
         <v>2</v>
       </c>
     </row>
@@ -3949,7 +3957,7 @@
       <c r="A12" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12">
         <v>1</v>
       </c>
     </row>
@@ -3957,7 +3965,7 @@
       <c r="A13" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13">
         <v>8</v>
       </c>
     </row>
@@ -3965,7 +3973,7 @@
       <c r="A14" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
T59v4 done with all statements, colorization Ok (for valid code)
</commit_message>
<xml_diff>
--- a/11_Grammars/Ti Docs/TI5x instructions.xlsx
+++ b/11_Grammars/Ti Docs/TI5x instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Projects\11_Grammars\Ti Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886E6756-4164-48C0-BF2C-E749B7D9EFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763049B8-1E65-4C5E-85CB-B515DA102B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="3840" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
+    <workbookView xWindow="24000" yWindow="11520" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions table" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="215">
   <si>
     <t>I11_a</t>
   </si>
@@ -652,9 +652,6 @@
   </si>
   <si>
     <t>X (Atomic inverse)</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Indirectible</t>
@@ -2211,7 +2208,8 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q102" sqref="Q102"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2239,7 @@
         <v>200</v>
       </c>
       <c r="F1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2531,7 +2529,7 @@
         <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,7 +2544,7 @@
         <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,6 +2561,9 @@
       <c r="D25" t="s">
         <v>184</v>
       </c>
+      <c r="E25" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2606,7 +2607,7 @@
         <v>109</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2687,7 +2688,7 @@
         <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2762,10 +2763,10 @@
         <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2834,7 +2835,7 @@
         <v>119</v>
       </c>
       <c r="D42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2849,7 +2850,7 @@
         <v>120</v>
       </c>
       <c r="D43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2864,10 +2865,10 @@
         <v>121</v>
       </c>
       <c r="D44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2882,10 +2883,10 @@
         <v>122</v>
       </c>
       <c r="D45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2900,13 +2901,13 @@
         <v>123</v>
       </c>
       <c r="D46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E46" t="s">
         <v>201</v>
       </c>
       <c r="F46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2923,6 +2924,9 @@
       <c r="D47" t="s">
         <v>184</v>
       </c>
+      <c r="E47" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -2936,7 +2940,7 @@
         <v>124</v>
       </c>
       <c r="D48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,10 +2970,10 @@
         <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2984,13 +2988,13 @@
         <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E51" t="s">
         <v>201</v>
       </c>
       <c r="F51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3020,7 +3024,7 @@
         <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3098,7 +3102,7 @@
         <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3188,7 +3192,7 @@
         <v>186</v>
       </c>
       <c r="F63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3206,7 +3210,7 @@
         <v>187</v>
       </c>
       <c r="F64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3224,7 +3228,7 @@
         <v>187</v>
       </c>
       <c r="F65" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -3245,7 +3249,7 @@
         <v>201</v>
       </c>
       <c r="F66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3326,10 +3330,10 @@
         <v>142</v>
       </c>
       <c r="D71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,7 +3387,7 @@
         <v>187</v>
       </c>
       <c r="F74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3401,7 +3405,7 @@
         <v>187</v>
       </c>
       <c r="F75" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3422,7 +3426,7 @@
         <v>201</v>
       </c>
       <c r="F76" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3569,7 +3573,7 @@
         <v>187</v>
       </c>
       <c r="F85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3587,7 +3591,7 @@
         <v>187</v>
       </c>
       <c r="F86" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3617,7 +3621,7 @@
         <v>155</v>
       </c>
       <c r="D88" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E88" t="s">
         <v>201</v>
@@ -3638,13 +3642,13 @@
         <v>156</v>
       </c>
       <c r="D89" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E89" t="s">
         <v>201</v>
       </c>
       <c r="F89" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3803,13 +3807,13 @@
         <v>162</v>
       </c>
       <c r="D99" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E99" t="s">
         <v>201</v>
       </c>
       <c r="F99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3826,9 +3830,7 @@
       <c r="D100" t="s">
         <v>184</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -3843,9 +3845,6 @@
       </c>
       <c r="D101" t="s">
         <v>184</v>
-      </c>
-      <c r="E101" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3883,10 +3882,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3907,7 +3906,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3915,7 +3914,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3939,7 +3938,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -3947,7 +3946,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -3971,7 +3970,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14">
         <v>100</v>

</xml_diff>

<commit_message>
Moved L2Inst to L1Tokenizer; Prepare L2Parser
</commit_message>
<xml_diff>
--- a/11_Grammars/Ti Docs/TI5x instructions.xlsx
+++ b/11_Grammars/Ti Docs/TI5x instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Projects\11_Grammars\Ti Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8038B7CA-7647-47DB-84AB-F16EC9D50578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052DFCF2-7590-400B-BC00-5154BB95211A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27645" yWindow="4725" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
+    <workbookView xWindow="4650" yWindow="6555" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions table" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="215">
   <si>
     <t>I11_a</t>
   </si>
@@ -522,9 +522,6 @@
     <t>x²|x^2|X2</t>
   </si>
   <si>
-    <t>^|y^x|YX|**</t>
-  </si>
-  <si>
     <t>|x||ABS|IXI</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>Grad|GRD</t>
   </si>
   <si>
-    <t>DMS|D.MS</t>
-  </si>
-  <si>
     <t>π|PI</t>
   </si>
   <si>
@@ -639,9 +633,6 @@
     <t>Count of Mnemonics</t>
   </si>
   <si>
-    <t>x&lt;&gt;t|x/t|x-t|x~t</t>
-  </si>
-  <si>
     <t>√|√x|SQRT</t>
   </si>
   <si>
@@ -685,6 +676,18 @@
   </si>
   <si>
     <t>IndMerged</t>
+  </si>
+  <si>
+    <t>D.MS|DMS</t>
+  </si>
+  <si>
+    <t>x⇄t|x↔t|x≷t|x&lt;&gt;t|x/t|x-t|x~t</t>
+  </si>
+  <si>
+    <t>yˣ|^|y^x|YX|**</t>
+  </si>
+  <si>
+    <t>p: prefix</t>
   </si>
 </sst>
 </file>
@@ -2215,18 +2218,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740F8AED-F224-4E04-9363-190526C87892}">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12:N101"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -2244,19 +2247,19 @@
         <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2264,10 +2267,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2275,10 +2278,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2286,10 +2289,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2297,10 +2300,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2308,10 +2311,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2319,10 +2322,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2330,10 +2333,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2341,10 +2344,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2352,10 +2355,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2363,10 +2366,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2381,11 +2384,11 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H12" t="str">
-        <f>IF(NOT(OR(ISBLANK(B12),ISBLANK(D12))), "tinst.Add(Vocab." &amp; B12&amp; ", new Inst{s=""" &amp; _xlfn.TEXTBEFORE(D12,":") &amp; """" &amp; IF(E12,", i=true","") &amp; IF(ISNUMBER(F12),", m=" &amp; F12,"") &amp; "});", "")</f>
-        <v>tinst.Add(Vocab.I10_e_prime, new Inst{s="a"});</v>
+        <f>IF(NOT(OR(ISBLANK(B12),ISBLANK(D12))), "TInst.Add(Vocab." &amp; B12&amp; ", new L1Inst{op=" &amp; MID(_xlfn.TEXTBEFORE(B12,"_"),2,999) &amp; ", m=""" &amp; _xlfn.TEXTBEFORE(C12&amp;"|","|") &amp; """, s=""" &amp; _xlfn.TEXTBEFORE(D12,":") &amp; """" &amp; IF(E12,", i=true","") &amp; IF(ISNUMBER(F12),", mop=" &amp; F12,"") &amp; "});", "")</f>
+        <v>TInst.Add(Vocab.I10_e_prime, new L1Inst{op=10, m="E'", s="a"});</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2400,11 +2403,11 @@
         <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" ref="H13:H76" si="1">IF(NOT(OR(ISBLANK(B13),ISBLANK(D13))), "tinst.Add(Vocab." &amp; B13&amp; ", new Inst{s=""" &amp; _xlfn.TEXTBEFORE(D13,":") &amp; """" &amp; IF(E13,", i=true","") &amp; IF(ISNUMBER(F13),", m=" &amp; F13,"") &amp; "});", "")</f>
-        <v>tinst.Add(Vocab.I11_a, new Inst{s="a"});</v>
+        <f t="shared" ref="H13:H76" si="1">IF(NOT(OR(ISBLANK(B13),ISBLANK(D13))), "TInst.Add(Vocab." &amp; B13&amp; ", new L1Inst{op=" &amp; MID(_xlfn.TEXTBEFORE(B13,"_"),2,999) &amp; ", m=""" &amp; _xlfn.TEXTBEFORE(C13&amp;"|","|") &amp; """, s=""" &amp; _xlfn.TEXTBEFORE(D13,":") &amp; """" &amp; IF(E13,", i=true","") &amp; IF(ISNUMBER(F13),", mop=" &amp; F13,"") &amp; "});", "")</f>
+        <v>TInst.Add(Vocab.I11_a, new L1Inst{op=11, m="A", s="a"});</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2419,11 +2422,11 @@
         <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I12_b, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I12_b, new L1Inst{op=12, m="B", s="a"});</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2438,11 +2441,11 @@
         <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I13_c, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I13_c, new L1Inst{op=13, m="C", s="a"});</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2457,14 +2460,14 @@
         <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I14_d, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I14_d, new L1Inst{op=14, m="D", s="a"});</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2476,14 +2479,14 @@
         <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I15_e, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I15_e, new L1Inst{op=15, m="E", s="a"});</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2495,14 +2498,14 @@
         <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I16_a_prime, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I16_a_prime, new L1Inst{op=16, m="A'", s="a"});</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2514,14 +2517,14 @@
         <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I17_b_prime, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I17_b_prime, new L1Inst{op=17, m="B'", s="a"});</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2533,14 +2536,14 @@
         <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I18_c_prime, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I18_c_prime, new L1Inst{op=18, m="C'", s="a"});</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2552,14 +2555,14 @@
         <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I19_d_prime, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I19_d_prime, new L1Inst{op=19, m="D'", s="a"});</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2571,14 +2574,14 @@
         <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I20_2nd_clear, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I20_2nd_clear, new L1Inst{op=20, m="CLR'", s="a"});</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2597,8 +2600,12 @@
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2610,17 +2617,17 @@
         <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G24" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I22_invert, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I22_invert, new L1Inst{op=22, m="INV", s="a"});</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2632,17 +2639,17 @@
         <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E25" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I23_ln, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I23_ln, new L1Inst{op=23, m="lnx", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2654,14 +2661,14 @@
         <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I24_correct_entry, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I24_correct_entry, new L1Inst{op=24, m="CE", s="a"});</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2673,14 +2680,14 @@
         <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I25_clear, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I25_clear, new L1Inst{op=25, m="CLR", s="a"});</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2699,8 +2706,12 @@
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2712,14 +2723,14 @@
         <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I27_2nd_invert, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I27_2nd_invert, new L1Inst{op=27, m="INV'", s="a"});</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2731,17 +2742,17 @@
         <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E30" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I28_log, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I28_log, new L1Inst{op=28, m="log", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2753,14 +2764,14 @@
         <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I29_clear_program, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I29_clear_program, new L1Inst{op=29, m="CP", s="a"});</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2772,17 +2783,17 @@
         <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E32" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I30_tan, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I30_tan, new L1Inst{op=30, m="tan", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2801,8 +2812,12 @@
       <c r="L33"/>
       <c r="M33"/>
       <c r="N33"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2811,17 +2826,17 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="D34" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I32_exchange_x_and_t, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I32_exchange_x_and_t, new L1Inst{op=32, m="x⇄t", s="a"});</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2833,14 +2848,14 @@
         <v>158</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I33_square, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I33_square, new L1Inst{op=33, m="x²", s="a"});</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2849,17 +2864,17 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I34_square_root, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I34_square_root, new L1Inst{op=34, m="√", s="a"});</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2871,14 +2886,14 @@
         <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I35_reciprocal, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I35_reciprocal, new L1Inst{op=35, m="1/x", s="a"});</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2890,17 +2905,17 @@
         <v>113</v>
       </c>
       <c r="D38" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F38" s="5">
         <v>62</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I36_program, new Inst{s="di", m=62});</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I36_program, new L1Inst{op=36, m="Pgm", s="di", mop=62});</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2909,20 +2924,20 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D39" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E39" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I37_polar_to_rectangular, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I37_polar_to_rectangular, new L1Inst{op=37, m="P-&gt;R", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2934,17 +2949,17 @@
         <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E40" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I38_sin, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I38_sin, new L1Inst{op=38, m="sin", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2956,17 +2971,17 @@
         <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E41" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I39_cos, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I39_cos, new L1Inst{op=39, m="cos", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2977,15 +2992,18 @@
       <c r="C42" t="s">
         <v>116</v>
       </c>
+      <c r="D42" t="s">
+        <v>214</v>
+      </c>
       <c r="G42" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I40_indirect, new L1Inst{op=40, m="Ind", s="p"});</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3004,8 +3022,12 @@
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ref="A44:A75" si="2">VALUE(MID(B44,2,2))</f>
         <v>42</v>
@@ -3017,17 +3039,17 @@
         <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F44" s="5">
         <v>72</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I42_store, new Inst{s="di", m=72});</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I42_store, new L1Inst{op=42, m="STO", s="di", mop=72});</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -3039,17 +3061,17 @@
         <v>118</v>
       </c>
       <c r="D45" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F45" s="5">
         <v>73</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I43_recall, new Inst{s="di", m=73});</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I43_recall, new L1Inst{op=43, m="RCL", s="di", mop=73});</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -3061,7 +3083,7 @@
         <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E46" s="5" t="b">
         <v>1</v>
@@ -3071,10 +3093,10 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I44_sum, new Inst{s="di", i=true, m=74});</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I44_sum, new L1Inst{op=44, m="SUM", s="di", i=true, mop=74});</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -3083,20 +3105,20 @@
         <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="D47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E47" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I45_power, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I45_power, new L1Inst{op=45, m="yˣ", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -3115,8 +3137,12 @@
       <c r="L48"/>
       <c r="M48"/>
       <c r="N48"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -3128,14 +3154,14 @@
         <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I47_clear_memory, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I47_clear_memory, new L1Inst{op=47, m="CMs", s="a"});</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -3147,17 +3173,17 @@
         <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F50" s="5">
         <v>63</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I48_exchange, new Inst{s="di", m=63});</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I48_exchange, new L1Inst{op=48, m="Exc", s="di", mop=63});</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -3169,7 +3195,7 @@
         <v>122</v>
       </c>
       <c r="D51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E51" s="5" t="b">
         <v>1</v>
@@ -3179,10 +3205,10 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I49_product, new Inst{s="di", i=true, m=64});</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I49_product, new L1Inst{op=49, m="Prd", s="di", i=true, mop=64});</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -3191,17 +3217,17 @@
         <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I50_absolute, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I50_absolute, new L1Inst{op=50, m="", s="a"});</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -3220,8 +3246,12 @@
       <c r="L53"/>
       <c r="M53"/>
       <c r="N53"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -3233,17 +3263,17 @@
         <v>123</v>
       </c>
       <c r="D54" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E54" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I52_exponent, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I52_exponent, new L1Inst{op=52, m="EE", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -3255,14 +3285,14 @@
         <v>124</v>
       </c>
       <c r="D55" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I53_left_parenthesis, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I53_left_parenthesis, new L1Inst{op=53, m="(", s="a"});</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -3274,14 +3304,14 @@
         <v>125</v>
       </c>
       <c r="D56" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I54_right_parenthesis, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I54_right_parenthesis, new L1Inst{op=54, m=")", s="a"});</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -3290,17 +3320,17 @@
         <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D57" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I55_divide, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I55_divide, new L1Inst{op=55, m="/", s="a"});</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -3319,8 +3349,12 @@
       <c r="L58"/>
       <c r="M58"/>
       <c r="N58"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -3332,17 +3366,17 @@
         <v>126</v>
       </c>
       <c r="D59" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E59" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I57_engineering, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I57_engineering, new L1Inst{op=57, m="Eng", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -3354,20 +3388,20 @@
         <v>127</v>
       </c>
       <c r="D60" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E60" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I58_fix, new Inst{s="di", i=true});</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I58_fix, new L1Inst{op=58, m="Fix", s="di", i=true});</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -3379,17 +3413,17 @@
         <v>128</v>
       </c>
       <c r="D61" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E61" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I59_integer, new Inst{s="a", i=true});</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I59_integer, new L1Inst{op=59, m="Int", s="a", i=true});</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -3401,14 +3435,14 @@
         <v>129</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I60_degrees, new Inst{s="a"});</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I60_degrees, new L1Inst{op=60, m="Deg", s="a"});</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -3420,17 +3454,17 @@
         <v>130</v>
       </c>
       <c r="D63" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F63" s="5">
         <v>83</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I61_goto, new Inst{s="b", m=83});</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+        <v>TInst.Add(Vocab.I61_goto, new L1Inst{op=61, m="GTO", s="b", mop=83});</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -3442,11 +3476,11 @@
         <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I62_program_indirect, new Inst{s="i"});</v>
+        <v>TInst.Add(Vocab.I62_program_indirect, new L1Inst{op=62, m="PG*", s="i"});</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3461,11 +3495,11 @@
         <v>132</v>
       </c>
       <c r="D65" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I63_exchange_indirect, new Inst{s="i"});</v>
+        <v>TInst.Add(Vocab.I63_exchange_indirect, new L1Inst{op=63, m="EX*", s="i"});</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3480,14 +3514,14 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E66" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I64_product_indirect, new Inst{s="i", i=true});</v>
+        <v>TInst.Add(Vocab.I64_product_indirect, new L1Inst{op=64, m="PD*", s="i", i=true});</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3499,14 +3533,14 @@
         <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I65_multiply, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I65_multiply, new L1Inst{op=65, m="*", s="a"});</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3518,14 +3552,14 @@
         <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D68" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I66_pause, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I66_pause, new L1Inst{op=66, m="Pause", s="a"});</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3537,17 +3571,17 @@
         <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D69" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E69" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I67_x_equals_t, new Inst{s="b", i=true});</v>
+        <v>TInst.Add(Vocab.I67_x_equals_t, new L1Inst{op=67, m="x=t", s="b", i=true});</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3562,11 +3596,11 @@
         <v>134</v>
       </c>
       <c r="D70" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I68_nop, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I68_nop, new L1Inst{op=68, m="Nop", s="a"});</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,14 +3615,14 @@
         <v>135</v>
       </c>
       <c r="D71" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F71" s="5">
         <v>84</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I69_operation, new Inst{s="di", m=84});</v>
+        <v>TInst.Add(Vocab.I69_operation, new L1Inst{op=69, m="Op", s="di", mop=84});</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3603,11 +3637,11 @@
         <v>136</v>
       </c>
       <c r="D72" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I70_radians, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I70_radians, new L1Inst{op=70, m="Rad", s="a"});</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3622,17 +3656,17 @@
         <v>137</v>
       </c>
       <c r="D73" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E73" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I71_subroutine, new Inst{s="b", i=true});</v>
+        <v>TInst.Add(Vocab.I71_subroutine, new L1Inst{op=71, m="SBR", s="b", i=true});</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3647,11 +3681,11 @@
         <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I72_store_indirect, new Inst{s="i"});</v>
+        <v>TInst.Add(Vocab.I72_store_indirect, new L1Inst{op=72, m="ST*", s="i"});</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3666,11 +3700,11 @@
         <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I73_recall_indirect, new Inst{s="i"});</v>
+        <v>TInst.Add(Vocab.I73_recall_indirect, new L1Inst{op=73, m="RC*", s="i"});</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3685,14 +3719,14 @@
         <v>140</v>
       </c>
       <c r="D76" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E76" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>tinst.Add(Vocab.I74_sum_indirect, new Inst{s="i", i=true});</v>
+        <v>TInst.Add(Vocab.I74_sum_indirect, new L1Inst{op=74, m="SM*", s="i", i=true});</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3707,11 +3741,11 @@
         <v>141</v>
       </c>
       <c r="D77" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" ref="H77:H101" si="4">IF(NOT(OR(ISBLANK(B77),ISBLANK(D77))), "tinst.Add(Vocab." &amp; B77&amp; ", new Inst{s=""" &amp; _xlfn.TEXTBEFORE(D77,":") &amp; """" &amp; IF(E77,", i=true","") &amp; IF(ISNUMBER(F77),", m=" &amp; F77,"") &amp; "});", "")</f>
-        <v>tinst.Add(Vocab.I75_subtract, new Inst{s="a"});</v>
+        <f t="shared" ref="H77:H101" si="4">IF(NOT(OR(ISBLANK(B77),ISBLANK(D77))), "TInst.Add(Vocab." &amp; B77&amp; ", new L1Inst{op=" &amp; MID(_xlfn.TEXTBEFORE(B77,"_"),2,999) &amp; ", m=""" &amp; _xlfn.TEXTBEFORE(C77&amp;"|","|") &amp; """, s=""" &amp; _xlfn.TEXTBEFORE(D77,":") &amp; """" &amp; IF(E77,", i=true","") &amp; IF(ISNUMBER(F77),", mop=" &amp; F77,"") &amp; "});", "")</f>
+        <v>TInst.Add(Vocab.I75_subtract, new L1Inst{op=75, m="-", s="a"});</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3726,11 +3760,11 @@
         <v>142</v>
       </c>
       <c r="D78" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I76_label, new Inst{s="m"});</v>
+        <v>TInst.Add(Vocab.I76_label, new L1Inst{op=76, m="Lbl", s="m"});</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3742,14 +3776,14 @@
         <v>66</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D79" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I77_x_greater_or_equal_than_t, new Inst{s="b"});</v>
+        <v>TInst.Add(Vocab.I77_x_greater_or_equal_than_t, new L1Inst{op=77, m="x≥t", s="b"});</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3761,17 +3795,17 @@
         <v>67</v>
       </c>
       <c r="C80" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E80" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I78_sigma_plus, new Inst{s="a", i=true});</v>
+        <v>TInst.Add(Vocab.I78_sigma_plus, new L1Inst{op=78, m="Σ+", s="a", i=true});</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3783,17 +3817,17 @@
         <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D81" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E81" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I79_average, new Inst{s="a", i=true});</v>
+        <v>TInst.Add(Vocab.I79_average, new L1Inst{op=79, m="x̄", s="a", i=true});</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3805,14 +3839,14 @@
         <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D82" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I80_grades, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I80_grades, new L1Inst{op=80, m="Grad", s="a"});</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3827,11 +3861,11 @@
         <v>143</v>
       </c>
       <c r="D83" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I81_reset, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I81_reset, new L1Inst{op=81, m="RST", s="a"});</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3846,11 +3880,11 @@
         <v>144</v>
       </c>
       <c r="D84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I82_hir, new Inst{s="d"});</v>
+        <v>TInst.Add(Vocab.I82_hir, new L1Inst{op=82, m="HIR", s="d"});</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,11 +3899,11 @@
         <v>145</v>
       </c>
       <c r="D85" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I83_goto_indirect, new Inst{s="i"});</v>
+        <v>TInst.Add(Vocab.I83_goto_indirect, new L1Inst{op=83, m="GO*", s="i"});</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3884,11 +3918,11 @@
         <v>146</v>
       </c>
       <c r="D86" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I84_operation_indirect, new Inst{s="i"});</v>
+        <v>TInst.Add(Vocab.I84_operation_indirect, new L1Inst{op=84, m="Op*", s="i"});</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3903,11 +3937,11 @@
         <v>147</v>
       </c>
       <c r="D87" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I85_add, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I85_add, new L1Inst{op=85, m="+", s="a"});</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3922,14 +3956,14 @@
         <v>148</v>
       </c>
       <c r="D88" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E88" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I86_set_flag, new Inst{s="di", i=true});</v>
+        <v>TInst.Add(Vocab.I86_set_flag, new L1Inst{op=86, m="STF", s="di", i=true});</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3944,14 +3978,14 @@
         <v>149</v>
       </c>
       <c r="D89" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E89" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I87_if_flag, new Inst{s="idb", i=true});</v>
+        <v>TInst.Add(Vocab.I87_if_flag, new L1Inst{op=87, m="IFF", s="idb", i=true});</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3963,17 +3997,17 @@
         <v>77</v>
       </c>
       <c r="C90" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="D90" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E90" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I88_dms, new Inst{s="a", i=true});</v>
+        <v>TInst.Add(Vocab.I88_dms, new L1Inst{op=88, m="D.MS", s="a", i=true});</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3985,14 +4019,14 @@
         <v>78</v>
       </c>
       <c r="C91" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D91" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I89_pi, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I89_pi, new L1Inst{op=89, m="π", s="a"});</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4004,17 +4038,17 @@
         <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D92" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E92" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I90_list, new Inst{s="a", i=true});</v>
+        <v>TInst.Add(Vocab.I90_list, new L1Inst{op=90, m="List", s="a", i=true});</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4029,11 +4063,11 @@
         <v>150</v>
       </c>
       <c r="D93" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I91_run_stop, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I91_run_stop, new L1Inst{op=91, m="R/S", s="a"});</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4048,11 +4082,11 @@
         <v>151</v>
       </c>
       <c r="D94" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I92_return, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I92_return, new L1Inst{op=92, m="RTN", s="a"});</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4067,11 +4101,11 @@
         <v>152</v>
       </c>
       <c r="D95" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I93_dot, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I93_dot, new L1Inst{op=93, m=".", s="a"});</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4086,11 +4120,11 @@
         <v>153</v>
       </c>
       <c r="D96" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I94_change_sign, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I94_change_sign, new L1Inst{op=94, m="+/-", s="a"});</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4105,11 +4139,11 @@
         <v>154</v>
       </c>
       <c r="D97" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I95_equals, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I95_equals, new L1Inst{op=95, m="=", s="a"});</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4121,17 +4155,17 @@
         <v>85</v>
       </c>
       <c r="C98" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D98" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E98" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I96_write, new Inst{s="a", i=true});</v>
+        <v>TInst.Add(Vocab.I96_write, new L1Inst{op=96, m="Write", s="a", i=true});</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4146,14 +4180,14 @@
         <v>155</v>
       </c>
       <c r="D99" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E99" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I97_dsz, new Inst{s="idb", i=true});</v>
+        <v>TInst.Add(Vocab.I97_dsz, new L1Inst{op=97, m="Dsz", s="idb", i=true});</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4168,13 +4202,13 @@
         <v>156</v>
       </c>
       <c r="D100" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E100" s="8"/>
       <c r="G100" s="1"/>
       <c r="H100" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I98_advance, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I98_advance, new L1Inst{op=98, m="Adv", s="a"});</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4189,11 +4223,11 @@
         <v>157</v>
       </c>
       <c r="D101" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="4"/>
-        <v>tinst.Add(Vocab.I99_print, new Inst{s="a"});</v>
+        <v>TInst.Add(Vocab.I99_print, new L1Inst{op=99, m="Prt", s="a"});</v>
       </c>
     </row>
   </sheetData>
@@ -4231,15 +4265,15 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" t="s">
         <v>195</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B4">
         <v>67</v>
@@ -4247,7 +4281,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -4255,7 +4289,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4263,7 +4297,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4271,7 +4305,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -4279,7 +4313,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4287,7 +4321,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -4295,7 +4329,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -4303,7 +4337,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4311,7 +4345,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -4319,7 +4353,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B14">
         <v>100</v>

</xml_diff>

<commit_message>
L2Parser almost good, only state dib remains to do
</commit_message>
<xml_diff>
--- a/11_Grammars/Ti Docs/TI5x instructions.xlsx
+++ b/11_Grammars/Ti Docs/TI5x instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Projects\11_Grammars\Ti Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052DFCF2-7590-400B-BC00-5154BB95211A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1492846-D8FE-41B9-972E-395CE274F34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4650" yWindow="6555" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
   </bookViews>
@@ -660,9 +660,6 @@
     <t>di: direct or indirect</t>
   </si>
   <si>
-    <t>idb: id, b</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -688,6 +685,9 @@
   </si>
   <si>
     <t>p: prefix</t>
+  </si>
+  <si>
+    <t>dib: di, b</t>
   </si>
 </sst>
 </file>
@@ -2221,8 +2221,8 @@
   <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,10 +2253,10 @@
         <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H1" t="s">
         <v>198</v>
@@ -2387,8 +2387,8 @@
         <v>199</v>
       </c>
       <c r="H12" t="str">
-        <f>IF(NOT(OR(ISBLANK(B12),ISBLANK(D12))), "TInst.Add(Vocab." &amp; B12&amp; ", new L1Inst{op=" &amp; MID(_xlfn.TEXTBEFORE(B12,"_"),2,999) &amp; ", m=""" &amp; _xlfn.TEXTBEFORE(C12&amp;"|","|") &amp; """, s=""" &amp; _xlfn.TEXTBEFORE(D12,":") &amp; """" &amp; IF(E12,", i=true","") &amp; IF(ISNUMBER(F12),", mop=" &amp; F12,"") &amp; "});", "")</f>
-        <v>TInst.Add(Vocab.I10_e_prime, new L1Inst{op=10, m="E'", s="a"});</v>
+        <f>IF(NOT(OR(ISBLANK(B12),ISBLANK(D12))), "TIKeys.Add(Vocab." &amp; B12&amp; ", new TIKey{Op=" &amp; MID(_xlfn.TEXTBEFORE(B12,"_"),2,999) &amp; ", M=""" &amp; _xlfn.TEXTBEFORE(C12&amp;"|","|") &amp; """, S=StatementSyntax." &amp; _xlfn.TEXTBEFORE(D12,":") &amp; IF(E12,", I=true","") &amp; IF(ISNUMBER(F12),", MOp=" &amp; F12,"") &amp; "});", "")</f>
+        <v>TIKeys.Add(Vocab.I10_e_prime, new TIKey{Op=10, M="E'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2406,8 +2406,8 @@
         <v>199</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" ref="H13:H76" si="1">IF(NOT(OR(ISBLANK(B13),ISBLANK(D13))), "TInst.Add(Vocab." &amp; B13&amp; ", new L1Inst{op=" &amp; MID(_xlfn.TEXTBEFORE(B13,"_"),2,999) &amp; ", m=""" &amp; _xlfn.TEXTBEFORE(C13&amp;"|","|") &amp; """, s=""" &amp; _xlfn.TEXTBEFORE(D13,":") &amp; """" &amp; IF(E13,", i=true","") &amp; IF(ISNUMBER(F13),", mop=" &amp; F13,"") &amp; "});", "")</f>
-        <v>TInst.Add(Vocab.I11_a, new L1Inst{op=11, m="A", s="a"});</v>
+        <f t="shared" ref="H13:H76" si="1">IF(NOT(OR(ISBLANK(B13),ISBLANK(D13))), "TIKeys.Add(Vocab." &amp; B13&amp; ", new TIKey{Op=" &amp; MID(_xlfn.TEXTBEFORE(B13,"_"),2,999) &amp; ", M=""" &amp; _xlfn.TEXTBEFORE(C13&amp;"|","|") &amp; """, S=StatementSyntax." &amp; _xlfn.TEXTBEFORE(D13,":") &amp; IF(E13,", I=true","") &amp; IF(ISNUMBER(F13),", MOp=" &amp; F13,"") &amp; "});", "")</f>
+        <v>TIKeys.Add(Vocab.I11_a, new TIKey{Op=11, M="A", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I12_b, new L1Inst{op=12, m="B", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I12_b, new TIKey{Op=12, M="B", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I13_c, new L1Inst{op=13, m="C", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I13_c, new TIKey{Op=13, M="C", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I14_d, new L1Inst{op=14, m="D", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I14_d, new TIKey{Op=14, M="D", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I15_e, new L1Inst{op=15, m="E", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I15_e, new TIKey{Op=15, M="E", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I16_a_prime, new L1Inst{op=16, m="A'", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I16_a_prime, new TIKey{Op=16, M="A'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I17_b_prime, new L1Inst{op=17, m="B'", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I17_b_prime, new TIKey{Op=17, M="B'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I18_c_prime, new L1Inst{op=18, m="C'", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I18_c_prime, new TIKey{Op=18, M="C'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I19_d_prime, new L1Inst{op=19, m="D'", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I19_d_prime, new TIKey{Op=19, M="D'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I20_2nd_clear, new L1Inst{op=20, m="CLR'", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I20_2nd_clear, new TIKey{Op=20, M="CLR'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2620,11 +2620,11 @@
         <v>199</v>
       </c>
       <c r="G24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I22_invert, new L1Inst{op=22, m="INV", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I22_invert, new TIKey{Op=22, M="INV", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I23_ln, new L1Inst{op=23, m="lnx", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I23_ln, new TIKey{Op=23, M="lnx", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I24_correct_entry, new L1Inst{op=24, m="CE", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I24_correct_entry, new TIKey{Op=24, M="CE", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2684,7 +2684,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I25_clear, new L1Inst{op=25, m="CLR", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I25_clear, new TIKey{Op=25, M="CLR", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="28" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I27_2nd_invert, new L1Inst{op=27, m="INV'", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I27_2nd_invert, new TIKey{Op=27, M="INV'", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I28_log, new L1Inst{op=28, m="log", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I28_log, new TIKey{Op=28, M="log", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I29_clear_program, new L1Inst{op=29, m="CP", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I29_clear_program, new TIKey{Op=29, M="CP", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I30_tan, new L1Inst{op=30, m="tan", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I30_tan, new TIKey{Op=30, M="tan", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2826,14 +2826,14 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D34" t="s">
         <v>199</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I32_exchange_x_and_t, new L1Inst{op=32, m="x⇄t", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I32_exchange_x_and_t, new TIKey{Op=32, M="x⇄t", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I33_square, new L1Inst{op=33, m="x²", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I33_square, new TIKey{Op=33, M="x²", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I34_square_root, new L1Inst{op=34, m="√", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I34_square_root, new TIKey{Op=34, M="√", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I35_reciprocal, new L1Inst{op=35, m="1/x", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I35_reciprocal, new TIKey{Op=35, M="1/x", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I36_program, new L1Inst{op=36, m="Pgm", s="di", mop=62});</v>
+        <v>TIKeys.Add(Vocab.I36_program, new TIKey{Op=36, M="Pgm", S=StatementSyntax.di, MOp=62});</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I37_polar_to_rectangular, new L1Inst{op=37, m="P-&gt;R", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I37_polar_to_rectangular, new TIKey{Op=37, M="P-&gt;R", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I38_sin, new L1Inst{op=38, m="sin", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I38_sin, new TIKey{Op=38, M="sin", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
       </c>
       <c r="H41" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I39_cos, new L1Inst{op=39, m="cos", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I39_cos, new TIKey{Op=39, M="cos", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -2993,14 +2993,14 @@
         <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I40_indirect, new L1Inst{op=40, m="Ind", s="p"});</v>
+        <v>TIKeys.Add(Vocab.I40_indirect, new TIKey{Op=40, M="Ind", S=StatementSyntax.p});</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I42_store, new L1Inst{op=42, m="STO", s="di", mop=72});</v>
+        <v>TIKeys.Add(Vocab.I42_store, new TIKey{Op=42, M="STO", S=StatementSyntax.di, MOp=72});</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I43_recall, new L1Inst{op=43, m="RCL", s="di", mop=73});</v>
+        <v>TIKeys.Add(Vocab.I43_recall, new TIKey{Op=43, M="RCL", S=StatementSyntax.di, MOp=73});</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I44_sum, new L1Inst{op=44, m="SUM", s="di", i=true, mop=74});</v>
+        <v>TIKeys.Add(Vocab.I44_sum, new TIKey{Op=44, M="SUM", S=StatementSyntax.di, I=true, MOp=74});</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
         <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D47" t="s">
         <v>199</v>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I45_power, new L1Inst{op=45, m="yˣ", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I45_power, new TIKey{Op=45, M="yˣ", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I47_clear_memory, new L1Inst{op=47, m="CMs", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I47_clear_memory, new TIKey{Op=47, M="CMs", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I48_exchange, new L1Inst{op=48, m="Exc", s="di", mop=63});</v>
+        <v>TIKeys.Add(Vocab.I48_exchange, new TIKey{Op=48, M="Exc", S=StatementSyntax.di, MOp=63});</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I49_product, new L1Inst{op=49, m="Prd", s="di", i=true, mop=64});</v>
+        <v>TIKeys.Add(Vocab.I49_product, new TIKey{Op=49, M="Prd", S=StatementSyntax.di, I=true, MOp=64});</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="H52" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I50_absolute, new L1Inst{op=50, m="", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I50_absolute, new TIKey{Op=50, M="", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="53" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3270,7 +3270,7 @@
       </c>
       <c r="H54" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I52_exponent, new L1Inst{op=52, m="EE", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I52_exponent, new TIKey{Op=52, M="EE", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -3289,7 +3289,7 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I53_left_parenthesis, new L1Inst{op=53, m="(", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I53_left_parenthesis, new TIKey{Op=53, M="(", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I54_right_parenthesis, new L1Inst{op=54, m=")", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I54_right_parenthesis, new TIKey{Op=54, M=")", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I55_divide, new L1Inst{op=55, m="/", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I55_divide, new TIKey{Op=55, M="/", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="58" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="H59" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I57_engineering, new L1Inst{op=57, m="Eng", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I57_engineering, new TIKey{Op=57, M="Eng", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -3394,11 +3394,11 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I58_fix, new L1Inst{op=58, m="Fix", s="di", i=true});</v>
+        <v>TIKeys.Add(Vocab.I58_fix, new TIKey{Op=58, M="Fix", S=StatementSyntax.di, I=true});</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3420,7 +3420,7 @@
       </c>
       <c r="H61" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I59_integer, new L1Inst{op=59, m="Int", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I59_integer, new TIKey{Op=59, M="Int", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
       </c>
       <c r="H62" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I60_degrees, new L1Inst{op=60, m="Deg", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I60_degrees, new TIKey{Op=60, M="Deg", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="H63" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I61_goto, new L1Inst{op=61, m="GTO", s="b", mop=83});</v>
+        <v>TIKeys.Add(Vocab.I61_goto, new TIKey{Op=61, M="GTO", S=StatementSyntax.b, MOp=83});</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="H64" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I62_program_indirect, new L1Inst{op=62, m="PG*", s="i"});</v>
+        <v>TIKeys.Add(Vocab.I62_program_indirect, new TIKey{Op=62, M="PG*", S=StatementSyntax.i});</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3499,7 +3499,7 @@
       </c>
       <c r="H65" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I63_exchange_indirect, new L1Inst{op=63, m="EX*", s="i"});</v>
+        <v>TIKeys.Add(Vocab.I63_exchange_indirect, new TIKey{Op=63, M="EX*", S=StatementSyntax.i});</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="H66" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I64_product_indirect, new L1Inst{op=64, m="PD*", s="i", i=true});</v>
+        <v>TIKeys.Add(Vocab.I64_product_indirect, new TIKey{Op=64, M="PD*", S=StatementSyntax.i, I=true});</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="H67" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I65_multiply, new L1Inst{op=65, m="*", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I65_multiply, new TIKey{Op=65, M="*", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I66_pause, new L1Inst{op=66, m="Pause", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I66_pause, new TIKey{Op=66, M="Pause", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I67_x_equals_t, new L1Inst{op=67, m="x=t", s="b", i=true});</v>
+        <v>TIKeys.Add(Vocab.I67_x_equals_t, new TIKey{Op=67, M="x=t", S=StatementSyntax.b, I=true});</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I68_nop, new L1Inst{op=68, m="Nop", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I68_nop, new TIKey{Op=68, M="Nop", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I69_operation, new L1Inst{op=69, m="Op", s="di", mop=84});</v>
+        <v>TIKeys.Add(Vocab.I69_operation, new TIKey{Op=69, M="Op", S=StatementSyntax.di, MOp=84});</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I70_radians, new L1Inst{op=70, m="Rad", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I70_radians, new TIKey{Op=70, M="Rad", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3662,11 +3662,11 @@
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I71_subroutine, new L1Inst{op=71, m="SBR", s="b", i=true});</v>
+        <v>TIKeys.Add(Vocab.I71_subroutine, new TIKey{Op=71, M="SBR", S=StatementSyntax.b, I=true});</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I72_store_indirect, new L1Inst{op=72, m="ST*", s="i"});</v>
+        <v>TIKeys.Add(Vocab.I72_store_indirect, new TIKey{Op=72, M="ST*", S=StatementSyntax.i});</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I73_recall_indirect, new L1Inst{op=73, m="RC*", s="i"});</v>
+        <v>TIKeys.Add(Vocab.I73_recall_indirect, new TIKey{Op=73, M="RC*", S=StatementSyntax.i});</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3726,7 +3726,7 @@
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>TInst.Add(Vocab.I74_sum_indirect, new L1Inst{op=74, m="SM*", s="i", i=true});</v>
+        <v>TIKeys.Add(Vocab.I74_sum_indirect, new TIKey{Op=74, M="SM*", S=StatementSyntax.i, I=true});</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3744,8 +3744,8 @@
         <v>199</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" ref="H77:H101" si="4">IF(NOT(OR(ISBLANK(B77),ISBLANK(D77))), "TInst.Add(Vocab." &amp; B77&amp; ", new L1Inst{op=" &amp; MID(_xlfn.TEXTBEFORE(B77,"_"),2,999) &amp; ", m=""" &amp; _xlfn.TEXTBEFORE(C77&amp;"|","|") &amp; """, s=""" &amp; _xlfn.TEXTBEFORE(D77,":") &amp; """" &amp; IF(E77,", i=true","") &amp; IF(ISNUMBER(F77),", mop=" &amp; F77,"") &amp; "});", "")</f>
-        <v>TInst.Add(Vocab.I75_subtract, new L1Inst{op=75, m="-", s="a"});</v>
+        <f t="shared" ref="H77:H101" si="4">IF(NOT(OR(ISBLANK(B77),ISBLANK(D77))), "TIKeys.Add(Vocab." &amp; B77&amp; ", new TIKey{Op=" &amp; MID(_xlfn.TEXTBEFORE(B77,"_"),2,999) &amp; ", M=""" &amp; _xlfn.TEXTBEFORE(C77&amp;"|","|") &amp; """, S=StatementSyntax." &amp; _xlfn.TEXTBEFORE(D77,":") &amp; IF(E77,", I=true","") &amp; IF(ISNUMBER(F77),", MOp=" &amp; F77,"") &amp; "});", "")</f>
+        <v>TIKeys.Add(Vocab.I75_subtract, new TIKey{Op=75, M="-", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3764,7 +3764,7 @@
       </c>
       <c r="H78" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I76_label, new L1Inst{op=76, m="Lbl", s="m"});</v>
+        <v>TIKeys.Add(Vocab.I76_label, new TIKey{Op=76, M="Lbl", S=StatementSyntax.m});</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="H79" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I77_x_greater_or_equal_than_t, new L1Inst{op=77, m="x≥t", s="b"});</v>
+        <v>TIKeys.Add(Vocab.I77_x_greater_or_equal_than_t, new TIKey{Op=77, M="x≥t", S=StatementSyntax.b});</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H80" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I78_sigma_plus, new L1Inst{op=78, m="Σ+", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I78_sigma_plus, new TIKey{Op=78, M="Σ+", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="H81" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I79_average, new L1Inst{op=79, m="x̄", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I79_average, new TIKey{Op=79, M="x̄", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="H82" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I80_grades, new L1Inst{op=80, m="Grad", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I80_grades, new TIKey{Op=80, M="Grad", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="H83" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I81_reset, new L1Inst{op=81, m="RST", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I81_reset, new TIKey{Op=81, M="RST", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="H84" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I82_hir, new L1Inst{op=82, m="HIR", s="d"});</v>
+        <v>TIKeys.Add(Vocab.I82_hir, new TIKey{Op=82, M="HIR", S=StatementSyntax.d});</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="H85" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I83_goto_indirect, new L1Inst{op=83, m="GO*", s="i"});</v>
+        <v>TIKeys.Add(Vocab.I83_goto_indirect, new TIKey{Op=83, M="GO*", S=StatementSyntax.i});</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="H86" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I84_operation_indirect, new L1Inst{op=84, m="Op*", s="i"});</v>
+        <v>TIKeys.Add(Vocab.I84_operation_indirect, new TIKey{Op=84, M="Op*", S=StatementSyntax.i});</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="H87" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I85_add, new L1Inst{op=85, m="+", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I85_add, new TIKey{Op=85, M="+", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="H88" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I86_set_flag, new L1Inst{op=86, m="STF", s="di", i=true});</v>
+        <v>TIKeys.Add(Vocab.I86_set_flag, new TIKey{Op=86, M="STF", S=StatementSyntax.di, I=true});</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3978,14 +3978,14 @@
         <v>149</v>
       </c>
       <c r="D89" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="E89" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I87_if_flag, new L1Inst{op=87, m="IFF", s="idb", i=true});</v>
+        <v>TIKeys.Add(Vocab.I87_if_flag, new TIKey{Op=87, M="IFF", S=StatementSyntax.dib, I=true});</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3997,7 +3997,7 @@
         <v>77</v>
       </c>
       <c r="C90" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D90" t="s">
         <v>199</v>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="H90" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I88_dms, new L1Inst{op=88, m="D.MS", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I88_dms, new TIKey{Op=88, M="D.MS", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="H91" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I89_pi, new L1Inst{op=89, m="π", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I89_pi, new TIKey{Op=89, M="π", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="H92" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I90_list, new L1Inst{op=90, m="List", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I90_list, new TIKey{Op=90, M="List", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4067,7 +4067,7 @@
       </c>
       <c r="H93" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I91_run_stop, new L1Inst{op=91, m="R/S", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I91_run_stop, new TIKey{Op=91, M="R/S", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="H94" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I92_return, new L1Inst{op=92, m="RTN", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I92_return, new TIKey{Op=92, M="RTN", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="H95" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I93_dot, new L1Inst{op=93, m=".", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I93_dot, new TIKey{Op=93, M=".", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="H96" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I94_change_sign, new L1Inst{op=94, m="+/-", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I94_change_sign, new TIKey{Op=94, M="+/-", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="H97" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I95_equals, new L1Inst{op=95, m="=", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I95_equals, new TIKey{Op=95, M="=", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="H98" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I96_write, new L1Inst{op=96, m="Write", s="a", i=true});</v>
+        <v>TIKeys.Add(Vocab.I96_write, new TIKey{Op=96, M="Write", S=StatementSyntax.a, I=true});</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4180,14 +4180,14 @@
         <v>155</v>
       </c>
       <c r="D99" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="E99" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I97_dsz, new L1Inst{op=97, m="Dsz", s="idb", i=true});</v>
+        <v>TIKeys.Add(Vocab.I97_dsz, new TIKey{Op=97, M="Dsz", S=StatementSyntax.dib, I=true});</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4208,7 +4208,7 @@
       <c r="G100" s="1"/>
       <c r="H100" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I98_advance, new L1Inst{op=98, m="Adv", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I98_advance, new TIKey{Op=98, M="Adv", S=StatementSyntax.a});</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="H101" t="str">
         <f t="shared" si="4"/>
-        <v>TInst.Add(Vocab.I99_print, new L1Inst{op=99, m="Prt", s="a"});</v>
+        <v>TIKeys.Add(Vocab.I99_print, new TIKey{Op=99, M="Prt", S=StatementSyntax.a});</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L2Parser Ok so far, remain the status of extended instructions, and TAG as a statement
</commit_message>
<xml_diff>
--- a/11_Grammars/Ti Docs/TI5x instructions.xlsx
+++ b/11_Grammars/Ti Docs/TI5x instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Projects\11_Grammars\Ti Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1492846-D8FE-41B9-972E-395CE274F34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB79CF91-E86B-408C-9B65-D350F1868950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4650" yWindow="6555" windowWidth="24645" windowHeight="23520" xr2:uid="{874B4454-468C-42B1-9C93-511E4410BC3F}"/>
   </bookViews>
@@ -2221,8 +2221,8 @@
   <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>